<commit_message>
Clean up code for function to get the coordinates of each gene region.
</commit_message>
<xml_diff>
--- a/Nextflow_backup/ChIP experiment SRA data.xlsx
+++ b/Nextflow_backup/ChIP experiment SRA data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42a5ee813758fc42/ChIP-seq-enrichment-analysis/Nextflow_backup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{BD1A4864-E89D-437D-B598-B87429B5A4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABC68B96-F5C9-4202-B3A2-309691F224D1}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{BD1A4864-E89D-437D-B598-B87429B5A4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED485FDF-622C-4D80-9EB2-B9F62EA13857}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9795" yWindow="3435" windowWidth="16305" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="497">
   <si>
     <t>Experiment</t>
   </si>
@@ -1497,6 +1497,36 @@
   </si>
   <si>
     <t>SRR19375287</t>
+  </si>
+  <si>
+    <t>GSE146931</t>
+  </si>
+  <si>
+    <t>PRJNA608903</t>
+  </si>
+  <si>
+    <t>SRR11192628</t>
+  </si>
+  <si>
+    <t>SRR11192627</t>
+  </si>
+  <si>
+    <t>WIP1</t>
+  </si>
+  <si>
+    <t>SRR11192624</t>
+  </si>
+  <si>
+    <t>SRR11192623</t>
+  </si>
+  <si>
+    <t>WIP2</t>
+  </si>
+  <si>
+    <t>SRR11192636</t>
+  </si>
+  <si>
+    <t>SRR11192635</t>
   </si>
 </sst>
 </file>
@@ -2337,10 +2367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I196"/>
+  <dimension ref="A1:I199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="C199" sqref="C199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3843,6 +3873,9 @@
       <c r="F67" t="s">
         <v>36</v>
       </c>
+      <c r="H67" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
@@ -6692,7 +6725,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>476</v>
       </c>
@@ -6712,7 +6745,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>476</v>
       </c>
@@ -6732,7 +6765,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>476</v>
       </c>
@@ -6752,7 +6785,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>476</v>
       </c>
@@ -6770,6 +6803,75 @@
       </c>
       <c r="F196" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>487</v>
+      </c>
+      <c r="B197" t="s">
+        <v>488</v>
+      </c>
+      <c r="C197" t="s">
+        <v>489</v>
+      </c>
+      <c r="D197" t="s">
+        <v>490</v>
+      </c>
+      <c r="E197" t="s">
+        <v>11</v>
+      </c>
+      <c r="F197" t="s">
+        <v>491</v>
+      </c>
+      <c r="H197" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>487</v>
+      </c>
+      <c r="B198" t="s">
+        <v>488</v>
+      </c>
+      <c r="C198" t="s">
+        <v>492</v>
+      </c>
+      <c r="D198" t="s">
+        <v>493</v>
+      </c>
+      <c r="E198" t="s">
+        <v>11</v>
+      </c>
+      <c r="F198" t="s">
+        <v>494</v>
+      </c>
+      <c r="H198" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>487</v>
+      </c>
+      <c r="B199" t="s">
+        <v>488</v>
+      </c>
+      <c r="C199" t="s">
+        <v>495</v>
+      </c>
+      <c r="D199" t="s">
+        <v>496</v>
+      </c>
+      <c r="E199" t="s">
+        <v>11</v>
+      </c>
+      <c r="F199" t="s">
+        <v>494</v>
+      </c>
+      <c r="H199" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>